<commit_message>
Version 1.1 complete and ready for fab.
</commit_message>
<xml_diff>
--- a/board_v11/RGB_Station_v11_BOM_Microchip.xlsx
+++ b/board_v11/RGB_Station_v11_BOM_Microchip.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RGB_Station\board_v10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\RGB_Station\board_v11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="146">
   <si>
     <t>Approved</t>
   </si>
@@ -205,12 +205,6 @@
     <t>DO NOT POPULATE ANY PARTS BELOW THIS LINE</t>
   </si>
   <si>
-    <t>Hirose</t>
-  </si>
-  <si>
-    <t>Bill of Materials For Project RGB Station v1.0</t>
-  </si>
-  <si>
     <t>SeeedStudios</t>
   </si>
   <si>
@@ -235,15 +229,6 @@
     <t>C5, C12, C13</t>
   </si>
   <si>
-    <t>H125270CT-ND</t>
-  </si>
-  <si>
-    <t>ZX62-B-5PA(33)</t>
-  </si>
-  <si>
-    <t>CONN RCPT USB MICRO B SMD R/A</t>
-  </si>
-  <si>
     <t>401-1427-1-ND</t>
   </si>
   <si>
@@ -298,18 +283,6 @@
     <t>Stackpole</t>
   </si>
   <si>
-    <t>R4, R8,R11</t>
-  </si>
-  <si>
-    <t>RMCF0603JT1K00CT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0603JT1K00</t>
-  </si>
-  <si>
-    <t>RES 1K OHM 1/10W 5% 0603 SMD</t>
-  </si>
-  <si>
     <t>C2, C4, C6, C7, C8, C9, C10, C14</t>
   </si>
   <si>
@@ -439,13 +412,55 @@
     <t>PIC32MX270F256D-50I/ML</t>
   </si>
   <si>
-    <t>RGB Station v1.0 blank PCB</t>
-  </si>
-  <si>
-    <t>MCP131T-315E/LB</t>
-  </si>
-  <si>
     <t>MicrochipDirect</t>
+  </si>
+  <si>
+    <t>R4,R8,R11</t>
+  </si>
+  <si>
+    <t>R2, R3</t>
+  </si>
+  <si>
+    <t>RMCF0603JT100RCT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT100R</t>
+  </si>
+  <si>
+    <t>RES SMD 100 OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RMCF0603JT8K20CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0603JT8K20</t>
+  </si>
+  <si>
+    <t>RES SMD 8.2K OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>732-3155-1-ND</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB MICRO B R/A SMT</t>
+  </si>
+  <si>
+    <t>Wurth Electronics Inc.</t>
+  </si>
+  <si>
+    <t>629105136821</t>
+  </si>
+  <si>
+    <t>Bill of Materials For Project RGB Station v1.1</t>
+  </si>
+  <si>
+    <t>RGB Station v1.1 blank PCB</t>
+  </si>
+  <si>
+    <t>MCP131T-315E/TT</t>
+  </si>
+  <si>
+    <t>MCP131T-315E/TTCT-ND</t>
   </si>
 </sst>
 </file>
@@ -457,7 +472,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -544,6 +559,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -959,7 +979,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1213,7 +1233,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="9" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="10" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1296,6 +1315,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="9" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1650,10 +1680,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1692,7 +1722,7 @@
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="77" t="s">
-        <v>61</v>
+        <v>142</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1714,8 +1744,8 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="120"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="119"/>
       <c r="M3" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="17.25" customHeight="1">
@@ -1723,7 +1753,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="75">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1731,8 +1761,8 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="124"/>
-      <c r="L4" s="121"/>
+      <c r="K4" s="123"/>
+      <c r="L4" s="120"/>
       <c r="M4" s="6"/>
     </row>
     <row r="5" spans="1:13" ht="17.25" customHeight="1">
@@ -1748,8 +1778,8 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="121"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="120"/>
       <c r="M5" s="6"/>
     </row>
     <row r="6" spans="1:13" ht="17.25" customHeight="1">
@@ -1765,8 +1795,8 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="124"/>
-      <c r="L6" s="121"/>
+      <c r="K6" s="123"/>
+      <c r="L6" s="120"/>
       <c r="M6" s="6"/>
     </row>
     <row r="7" spans="1:13">
@@ -1778,8 +1808,8 @@
       <c r="H7" s="45"/>
       <c r="I7" s="59"/>
       <c r="J7" s="85"/>
-      <c r="K7" s="125"/>
-      <c r="L7" s="122"/>
+      <c r="K7" s="124"/>
+      <c r="L7" s="121"/>
       <c r="M7" s="60"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
@@ -1870,38 +1900,38 @@
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="C12" s="115">
+      <c r="C12" s="114">
         <v>1</v>
       </c>
       <c r="D12" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="112" t="s">
         <v>64</v>
-      </c>
-      <c r="E12" s="113" t="s">
-        <v>66</v>
       </c>
       <c r="F12" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="116" t="s">
-        <v>67</v>
-      </c>
-      <c r="H12" s="94" t="s">
+      <c r="G12" s="115" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="113" t="s">
-        <v>65</v>
+      <c r="I12" s="112" t="s">
+        <v>63</v>
       </c>
       <c r="J12" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="91">
-        <v>1</v>
-      </c>
-      <c r="L12" s="119">
+      <c r="K12" s="90">
+        <v>1</v>
+      </c>
+      <c r="L12" s="118">
         <v>0.88</v>
       </c>
       <c r="M12" s="54">
-        <f t="shared" ref="M12:M31" si="0">K12*L12</f>
+        <f t="shared" ref="M12:M32" si="0">K12*L12</f>
         <v>0.88</v>
       </c>
     </row>
@@ -1909,34 +1939,34 @@
       <c r="A13" s="8">
         <v>2</v>
       </c>
-      <c r="C13" s="115">
+      <c r="C13" s="114">
         <v>1</v>
       </c>
       <c r="D13" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="92" t="s">
+      <c r="E13" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="93" t="s">
+      <c r="F13" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="117" t="s">
+      <c r="G13" s="116" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="94" t="s">
+      <c r="H13" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="113" t="s">
-        <v>68</v>
+      <c r="I13" s="112" t="s">
+        <v>66</v>
       </c>
       <c r="J13" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K13" s="91">
-        <v>1</v>
-      </c>
-      <c r="L13" s="119">
+      <c r="K13" s="90">
+        <v>1</v>
+      </c>
+      <c r="L13" s="118">
         <v>0.5</v>
       </c>
       <c r="M13" s="54">
@@ -1948,34 +1978,34 @@
       <c r="A14" s="8">
         <v>1</v>
       </c>
-      <c r="C14" s="115">
+      <c r="C14" s="114">
         <v>1</v>
       </c>
       <c r="D14" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="92" t="s">
+      <c r="E14" s="91" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="93" t="s">
+      <c r="F14" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="118" t="s">
+      <c r="G14" s="117" t="s">
         <v>55</v>
       </c>
-      <c r="H14" s="94" t="s">
+      <c r="H14" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="96" t="s">
+      <c r="I14" s="95" t="s">
         <v>57</v>
       </c>
       <c r="J14" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="91">
-        <v>1</v>
-      </c>
-      <c r="L14" s="119">
+      <c r="K14" s="90">
+        <v>1</v>
+      </c>
+      <c r="L14" s="118">
         <v>0.1</v>
       </c>
       <c r="M14" s="54">
@@ -1987,34 +2017,34 @@
       <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="C15" s="115">
+      <c r="C15" s="114">
         <v>3</v>
       </c>
       <c r="D15" s="89" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="102" t="s">
-        <v>86</v>
-      </c>
-      <c r="G15" s="104" t="s">
-        <v>135</v>
-      </c>
-      <c r="H15" s="94" t="s">
+      <c r="F15" s="101" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="129" t="s">
+        <v>126</v>
+      </c>
+      <c r="H15" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="101" t="s">
-        <v>134</v>
+      <c r="I15" s="100" t="s">
+        <v>125</v>
       </c>
       <c r="J15" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="91">
+      <c r="K15" s="90">
         <v>3</v>
       </c>
-      <c r="L15" s="119">
+      <c r="L15" s="118">
         <v>0.15</v>
       </c>
       <c r="M15" s="54">
@@ -2026,73 +2056,73 @@
       <c r="A16" s="8">
         <v>1</v>
       </c>
-      <c r="C16" s="115">
+      <c r="C16" s="114">
         <v>1</v>
       </c>
       <c r="D16" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="113" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="93" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="116" t="s">
-        <v>71</v>
-      </c>
-      <c r="H16" s="94" t="s">
+      <c r="E16" s="128" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" s="113" t="s">
+        <v>140</v>
+      </c>
+      <c r="G16" s="130" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="113" t="s">
-        <v>70</v>
+      <c r="I16" s="100" t="s">
+        <v>138</v>
       </c>
       <c r="J16" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="91">
-        <v>1</v>
-      </c>
-      <c r="L16" s="119">
-        <v>0.84</v>
+      <c r="K16" s="90">
+        <v>1</v>
+      </c>
+      <c r="L16" s="118">
+        <v>1.21</v>
       </c>
       <c r="M16" s="54">
         <f t="shared" si="0"/>
-        <v>0.84</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="8" customFormat="1">
       <c r="A17" s="8">
         <v>1</v>
       </c>
-      <c r="C17" s="115">
+      <c r="C17" s="114">
         <v>2</v>
       </c>
       <c r="D17" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="113" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="93" t="s">
+      <c r="E17" s="128" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="101" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="H17" s="94" t="s">
+      <c r="G17" s="131" t="s">
+        <v>70</v>
+      </c>
+      <c r="H17" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="113" t="s">
-        <v>73</v>
+      <c r="I17" s="112" t="s">
+        <v>68</v>
       </c>
       <c r="J17" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="91">
+      <c r="K17" s="90">
         <v>2</v>
       </c>
-      <c r="L17" s="119">
+      <c r="L17" s="118">
         <v>0.51</v>
       </c>
       <c r="M17" s="54">
@@ -2104,34 +2134,34 @@
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="C18" s="115">
+      <c r="C18" s="114">
         <v>8</v>
       </c>
       <c r="D18" s="89" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="113" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="G18" s="116" t="s">
-        <v>85</v>
-      </c>
-      <c r="H18" s="94" t="s">
+      <c r="E18" s="128" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="101" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="131" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="113" t="s">
-        <v>84</v>
+      <c r="I18" s="112" t="s">
+        <v>79</v>
       </c>
       <c r="J18" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K18" s="91">
+      <c r="K18" s="90">
         <v>8</v>
       </c>
-      <c r="L18" s="119">
+      <c r="L18" s="118">
         <v>0.1</v>
       </c>
       <c r="M18" s="54">
@@ -2143,34 +2173,34 @@
       <c r="A19" s="8">
         <v>2</v>
       </c>
-      <c r="C19" s="115">
+      <c r="C19" s="114">
         <v>1</v>
       </c>
       <c r="D19" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="E19" s="113" t="s">
-        <v>105</v>
-      </c>
-      <c r="F19" s="102" t="s">
-        <v>102</v>
-      </c>
-      <c r="G19" s="116" t="s">
-        <v>104</v>
-      </c>
-      <c r="H19" s="94" t="s">
+      <c r="E19" s="128" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19" s="101" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" s="131" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I19" s="113" t="s">
-        <v>103</v>
+      <c r="I19" s="112" t="s">
+        <v>94</v>
       </c>
       <c r="J19" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="91">
-        <v>1</v>
-      </c>
-      <c r="L19" s="119">
+      <c r="K19" s="90">
+        <v>1</v>
+      </c>
+      <c r="L19" s="118">
         <v>0.14000000000000001</v>
       </c>
       <c r="M19" s="54">
@@ -2182,34 +2212,34 @@
       <c r="A20" s="8">
         <v>1</v>
       </c>
-      <c r="C20" s="115">
+      <c r="C20" s="114">
         <v>1</v>
       </c>
       <c r="D20" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="113" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="102" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20" s="116" t="s">
-        <v>107</v>
-      </c>
-      <c r="H20" s="94" t="s">
+      <c r="E20" s="128" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="101" t="s">
+        <v>93</v>
+      </c>
+      <c r="G20" s="131" t="s">
+        <v>98</v>
+      </c>
+      <c r="H20" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="113" t="s">
-        <v>106</v>
+      <c r="I20" s="112" t="s">
+        <v>97</v>
       </c>
       <c r="J20" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K20" s="91">
-        <v>1</v>
-      </c>
-      <c r="L20" s="119">
+      <c r="K20" s="90">
+        <v>1</v>
+      </c>
+      <c r="L20" s="118">
         <v>0.22</v>
       </c>
       <c r="M20" s="54">
@@ -2221,34 +2251,34 @@
       <c r="A21" s="8">
         <v>2</v>
       </c>
-      <c r="C21" s="115">
+      <c r="C21" s="114">
         <v>3</v>
       </c>
       <c r="D21" s="89" t="s">
-        <v>91</v>
-      </c>
-      <c r="E21" s="92" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="102" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="116" t="s">
-        <v>93</v>
-      </c>
-      <c r="H21" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="128" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="101" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="129" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="113" t="s">
-        <v>92</v>
+      <c r="I21" s="100" t="s">
+        <v>135</v>
       </c>
       <c r="J21" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="91">
+      <c r="K21" s="90">
         <v>3</v>
       </c>
-      <c r="L21" s="119">
+      <c r="L21" s="118">
         <v>0.1</v>
       </c>
       <c r="M21" s="54">
@@ -2260,34 +2290,34 @@
       <c r="A22" s="8">
         <v>1</v>
       </c>
-      <c r="C22" s="115">
+      <c r="C22" s="114">
         <v>3</v>
       </c>
-      <c r="D22" s="88" t="s">
+      <c r="D22" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="E22" s="92" t="s">
+      <c r="E22" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="102" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="116" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" s="94" t="s">
+      <c r="F22" s="101" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="131" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="113" t="s">
-        <v>88</v>
+      <c r="I22" s="112" t="s">
+        <v>83</v>
       </c>
       <c r="J22" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K22" s="91">
+      <c r="K22" s="90">
         <v>3</v>
       </c>
-      <c r="L22" s="119">
+      <c r="L22" s="118">
         <v>0.1</v>
       </c>
       <c r="M22" s="54">
@@ -2299,34 +2329,34 @@
       <c r="A23" s="8">
         <v>4</v>
       </c>
-      <c r="C23" s="115">
+      <c r="C23" s="114">
         <v>1</v>
       </c>
       <c r="D23" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="92" t="s">
+      <c r="E23" s="91" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="93" t="s">
+      <c r="F23" s="101" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="104" t="s">
-        <v>137</v>
-      </c>
-      <c r="H23" s="94" t="s">
+      <c r="G23" s="129" t="s">
+        <v>128</v>
+      </c>
+      <c r="H23" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="101" t="s">
-        <v>136</v>
+      <c r="I23" s="100" t="s">
+        <v>127</v>
       </c>
       <c r="J23" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K23" s="91">
-        <v>1</v>
-      </c>
-      <c r="L23" s="119">
+      <c r="K23" s="90">
+        <v>1</v>
+      </c>
+      <c r="L23" s="118">
         <v>4.6900000000000004</v>
       </c>
       <c r="M23" s="54">
@@ -2338,34 +2368,34 @@
       <c r="A24" s="8">
         <v>1</v>
       </c>
-      <c r="C24" s="115">
+      <c r="C24" s="114">
         <v>1</v>
       </c>
       <c r="D24" s="89" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="113" t="s">
-        <v>111</v>
-      </c>
-      <c r="F24" s="102" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="128" t="s">
         <v>102</v>
       </c>
-      <c r="G24" s="116" t="s">
-        <v>110</v>
-      </c>
-      <c r="H24" s="94" t="s">
+      <c r="F24" s="101" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="131" t="s">
+        <v>101</v>
+      </c>
+      <c r="H24" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I24" s="113" t="s">
-        <v>109</v>
+      <c r="I24" s="112" t="s">
+        <v>100</v>
       </c>
       <c r="J24" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K24" s="91">
-        <v>1</v>
-      </c>
-      <c r="L24" s="119">
+      <c r="K24" s="90">
+        <v>1</v>
+      </c>
+      <c r="L24" s="118">
         <v>0.15</v>
       </c>
       <c r="M24" s="54">
@@ -2377,32 +2407,32 @@
       <c r="A25" s="8">
         <v>1</v>
       </c>
-      <c r="C25" s="115">
-        <v>1</v>
-      </c>
-      <c r="D25" s="90"/>
-      <c r="E25" s="92" t="s">
-        <v>138</v>
-      </c>
-      <c r="F25" s="102" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="117" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" s="103" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="95" t="s">
-        <v>63</v>
+      <c r="C25" s="114">
+        <v>1</v>
+      </c>
+      <c r="D25" s="127"/>
+      <c r="E25" s="91" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="101" t="s">
+        <v>60</v>
+      </c>
+      <c r="G25" s="116" t="s">
+        <v>61</v>
+      </c>
+      <c r="H25" s="102" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="94" t="s">
+        <v>61</v>
       </c>
       <c r="J25" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K25" s="91">
-        <v>1</v>
-      </c>
-      <c r="L25" s="119"/>
+      <c r="K25" s="90">
+        <v>1</v>
+      </c>
+      <c r="L25" s="118"/>
       <c r="M25" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2412,34 +2442,34 @@
       <c r="A26" s="8">
         <v>2</v>
       </c>
-      <c r="C26" s="115">
+      <c r="C26" s="114">
         <v>1</v>
       </c>
       <c r="D26" s="89" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" s="113" t="s">
-        <v>116</v>
-      </c>
-      <c r="F26" s="114" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="116" t="s">
-        <v>115</v>
-      </c>
-      <c r="H26" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="128" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="113" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="131" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I26" s="113" t="s">
-        <v>113</v>
+      <c r="I26" s="112" t="s">
+        <v>104</v>
       </c>
       <c r="J26" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="91">
-        <v>1</v>
-      </c>
-      <c r="L26" s="119">
+      <c r="K26" s="90">
+        <v>1</v>
+      </c>
+      <c r="L26" s="118">
         <v>0.57999999999999996</v>
       </c>
       <c r="M26" s="54">
@@ -2448,34 +2478,34 @@
       </c>
     </row>
     <row r="27" spans="1:13" s="8" customFormat="1">
-      <c r="C27" s="115">
+      <c r="C27" s="114">
         <v>1</v>
       </c>
       <c r="D27" s="89" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" s="113" t="s">
-        <v>120</v>
-      </c>
-      <c r="F27" s="114" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="128" t="s">
+        <v>111</v>
+      </c>
+      <c r="F27" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="116" t="s">
-        <v>119</v>
-      </c>
-      <c r="H27" s="94" t="s">
+      <c r="G27" s="131" t="s">
+        <v>110</v>
+      </c>
+      <c r="H27" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I27" s="113" t="s">
-        <v>118</v>
+      <c r="I27" s="112" t="s">
+        <v>109</v>
       </c>
       <c r="J27" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K27" s="91">
-        <v>1</v>
-      </c>
-      <c r="L27" s="119">
+      <c r="K27" s="90">
+        <v>1</v>
+      </c>
+      <c r="L27" s="118">
         <v>7.38</v>
       </c>
       <c r="M27" s="54">
@@ -2484,70 +2514,70 @@
       </c>
     </row>
     <row r="28" spans="1:13" s="8" customFormat="1">
-      <c r="C28" s="115">
+      <c r="C28" s="114">
         <v>1</v>
       </c>
       <c r="D28" s="89" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28" s="113" t="s">
-        <v>122</v>
-      </c>
-      <c r="F28" s="114" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="112" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="113" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="104" t="s">
-        <v>139</v>
-      </c>
-      <c r="H28" s="94" t="s">
-        <v>140</v>
-      </c>
-      <c r="I28" s="104" t="s">
-        <v>139</v>
+      <c r="G28" s="103" t="s">
+        <v>144</v>
+      </c>
+      <c r="H28" s="93" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" s="100" t="s">
+        <v>145</v>
       </c>
       <c r="J28" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="91">
-        <v>1</v>
-      </c>
-      <c r="L28" s="119">
-        <v>0.5</v>
+      <c r="K28" s="90">
+        <v>1</v>
+      </c>
+      <c r="L28" s="118">
+        <v>0.53</v>
       </c>
       <c r="M28" s="54">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="8" customFormat="1">
-      <c r="C29" s="115">
+      <c r="C29" s="114">
         <v>1</v>
       </c>
       <c r="D29" s="89" t="s">
-        <v>123</v>
-      </c>
-      <c r="E29" s="113" t="s">
-        <v>126</v>
-      </c>
-      <c r="F29" s="114" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" s="112" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="113" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="116" t="s">
-        <v>125</v>
-      </c>
-      <c r="H29" s="94" t="s">
+      <c r="G29" s="115" t="s">
+        <v>116</v>
+      </c>
+      <c r="H29" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="113" t="s">
-        <v>124</v>
+      <c r="I29" s="112" t="s">
+        <v>115</v>
       </c>
       <c r="J29" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K29" s="91">
-        <v>1</v>
-      </c>
-      <c r="L29" s="119">
+      <c r="K29" s="90">
+        <v>1</v>
+      </c>
+      <c r="L29" s="118">
         <v>0.31</v>
       </c>
       <c r="M29" s="54">
@@ -2556,34 +2586,34 @@
       </c>
     </row>
     <row r="30" spans="1:13" s="8" customFormat="1">
-      <c r="C30" s="115">
+      <c r="C30" s="114">
         <v>1</v>
       </c>
       <c r="D30" s="89" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="113" t="s">
-        <v>130</v>
-      </c>
-      <c r="F30" s="114" t="s">
-        <v>129</v>
-      </c>
-      <c r="G30" s="116">
+        <v>118</v>
+      </c>
+      <c r="E30" s="112" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="G30" s="115">
         <v>1984617</v>
       </c>
-      <c r="H30" s="94" t="s">
+      <c r="H30" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="113" t="s">
-        <v>128</v>
+      <c r="I30" s="112" t="s">
+        <v>119</v>
       </c>
       <c r="J30" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="91">
-        <v>1</v>
-      </c>
-      <c r="L30" s="119">
+      <c r="K30" s="90">
+        <v>1</v>
+      </c>
+      <c r="L30" s="118">
         <v>0.43</v>
       </c>
       <c r="M30" s="54">
@@ -2592,34 +2622,34 @@
       </c>
     </row>
     <row r="31" spans="1:13" s="8" customFormat="1">
-      <c r="C31" s="115">
+      <c r="C31" s="114">
         <v>1</v>
       </c>
       <c r="D31" s="89" t="s">
-        <v>131</v>
-      </c>
-      <c r="E31" s="113" t="s">
-        <v>133</v>
-      </c>
-      <c r="F31" s="114" t="s">
-        <v>129</v>
-      </c>
-      <c r="G31" s="116">
+        <v>122</v>
+      </c>
+      <c r="E31" s="112" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" s="113" t="s">
+        <v>120</v>
+      </c>
+      <c r="G31" s="115">
         <v>1984633</v>
       </c>
-      <c r="H31" s="94" t="s">
+      <c r="H31" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="I31" s="113" t="s">
-        <v>132</v>
+      <c r="I31" s="112" t="s">
+        <v>123</v>
       </c>
       <c r="J31" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K31" s="91">
-        <v>1</v>
-      </c>
-      <c r="L31" s="119">
+      <c r="K31" s="90">
+        <v>1</v>
+      </c>
+      <c r="L31" s="118">
         <v>0.85</v>
       </c>
       <c r="M31" s="54">
@@ -2628,62 +2658,76 @@
       </c>
     </row>
     <row r="32" spans="1:13" s="8" customFormat="1">
-      <c r="A32" s="8">
-        <v>1</v>
-      </c>
-      <c r="C32" s="126" t="s">
+      <c r="C32" s="114">
+        <v>2</v>
+      </c>
+      <c r="D32" s="89" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="100" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="101" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="103" t="s">
+        <v>133</v>
+      </c>
+      <c r="H32" s="93" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="100" t="s">
+        <v>132</v>
+      </c>
+      <c r="J32" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="90">
+        <v>2</v>
+      </c>
+      <c r="L32" s="118">
+        <v>0.1</v>
+      </c>
+      <c r="M32" s="54">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="8" customFormat="1">
+      <c r="A33" s="8">
+        <v>1</v>
+      </c>
+      <c r="C33" s="125" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="127"/>
-      <c r="E32" s="127"/>
-      <c r="F32" s="127"/>
-      <c r="G32" s="127"/>
-      <c r="H32" s="80"/>
-      <c r="I32" s="80"/>
-      <c r="J32" s="53"/>
-      <c r="K32" s="53"/>
-      <c r="L32" s="119"/>
-      <c r="M32" s="54"/>
-    </row>
-    <row r="33" spans="1:13" s="8" customFormat="1">
-      <c r="C33" s="58">
-        <v>0</v>
-      </c>
-      <c r="D33" s="87" t="s">
-        <v>97</v>
-      </c>
-      <c r="E33" s="97" t="s">
-        <v>100</v>
-      </c>
-      <c r="F33" s="93"/>
-      <c r="G33" s="97"/>
-      <c r="H33" s="99"/>
-      <c r="I33" s="97"/>
+      <c r="D33" s="126"/>
+      <c r="E33" s="126"/>
+      <c r="F33" s="126"/>
+      <c r="G33" s="126"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
       <c r="J33" s="53"/>
       <c r="K33" s="53"/>
-      <c r="L33" s="119"/>
+      <c r="L33" s="118"/>
       <c r="M33" s="54"/>
     </row>
     <row r="34" spans="1:13" s="8" customFormat="1">
-      <c r="A34" s="8">
-        <v>1</v>
-      </c>
       <c r="C34" s="58">
         <v>0</v>
       </c>
       <c r="D34" s="87" t="s">
-        <v>98</v>
-      </c>
-      <c r="E34" s="98" t="s">
-        <v>99</v>
-      </c>
-      <c r="F34" s="93"/>
-      <c r="G34" s="98"/>
-      <c r="H34" s="100"/>
-      <c r="I34" s="98"/>
+        <v>88</v>
+      </c>
+      <c r="E34" s="96" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="92"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="96"/>
       <c r="J34" s="53"/>
       <c r="K34" s="53"/>
-      <c r="L34" s="119"/>
+      <c r="L34" s="118"/>
       <c r="M34" s="54"/>
     </row>
     <row r="35" spans="1:13" s="8" customFormat="1">
@@ -2694,80 +2738,89 @@
         <v>0</v>
       </c>
       <c r="D35" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="E35" s="102" t="s">
-        <v>101</v>
-      </c>
-      <c r="F35" s="80"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="80"/>
+        <v>89</v>
+      </c>
+      <c r="E35" s="97" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="92"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="97"/>
       <c r="J35" s="53"/>
       <c r="K35" s="53"/>
-      <c r="L35" s="119"/>
+      <c r="L35" s="118"/>
       <c r="M35" s="54"/>
     </row>
-    <row r="36" spans="1:13">
-      <c r="C36" s="48"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="50"/>
-      <c r="K36" s="50"/>
-      <c r="L36" s="50"/>
-      <c r="M36" s="52">
-        <f>SUM(M12:M35)</f>
-        <v>20.439999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" customFormat="1" ht="13.7" customHeight="1">
-      <c r="C37" s="35" t="s">
+    <row r="36" spans="1:13" s="8" customFormat="1">
+      <c r="A36" s="8">
+        <v>1</v>
+      </c>
+      <c r="C36" s="58">
         <v>0</v>
       </c>
-      <c r="D37" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="47"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="41" t="s">
+      <c r="D36" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="101" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="118"/>
+      <c r="M36" s="54"/>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="C37" s="48"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="52">
+        <f>SUM(M12:M36)</f>
+        <v>21.04</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" customFormat="1" ht="13.7" customHeight="1">
+      <c r="C38" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="41" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C38" s="38"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="51"/>
-      <c r="M38" s="68"/>
-    </row>
     <row r="39" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C39" s="36"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="69"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="68"/>
     </row>
     <row r="40" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
       <c r="C40" s="36"/>
@@ -2795,23 +2848,23 @@
       <c r="L41" s="27"/>
       <c r="M41" s="69"/>
     </row>
-    <row r="42" spans="1:13" customFormat="1" ht="9.75" customHeight="1">
-      <c r="C42" s="37"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
-      <c r="H42" s="29"/>
-      <c r="I42" s="29"/>
-      <c r="J42" s="29"/>
-      <c r="K42" s="29"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="70"/>
-    </row>
-    <row r="43" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+    <row r="42" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="C42" s="36"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="69"/>
+    </row>
+    <row r="43" spans="1:13" customFormat="1" ht="9.75" customHeight="1">
       <c r="C43" s="37"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="29"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="43"/>
       <c r="F43" s="29"/>
       <c r="G43" s="29"/>
       <c r="H43" s="29"/>
@@ -2819,46 +2872,60 @@
       <c r="J43" s="29"/>
       <c r="K43" s="29"/>
       <c r="L43" s="29"/>
-      <c r="M43" s="67"/>
+      <c r="M43" s="70"/>
     </row>
     <row r="44" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C44" s="16"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18"/>
-      <c r="M44" s="65"/>
+      <c r="C44" s="37"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="67"/>
     </row>
     <row r="45" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
-      <c r="C45" s="19"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="21"/>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="21"/>
-      <c r="M45" s="66"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="65"/>
+    </row>
+    <row r="46" spans="1:13" customFormat="1" ht="12.95" customHeight="1">
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="L3:L7"/>
     <mergeCell ref="K3:K7"/>
-    <mergeCell ref="C32:G32"/>
+    <mergeCell ref="C33:G33"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F26" r:id="rId1" display="https://www.digikey.com/en/supplier-centers/n/nexperia" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F16" r:id="rId2" display="https://www.digikey.com/en/supplier-centers/w/wurth-electronics" xr:uid="{932E3419-F0AF-4188-9299-2804C504F6FE}"/>
   </hyperlinks>
   <pageMargins left="0.46" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="17" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId2"/>
+  <pageSetup paperSize="17" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId3"/>
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;BAltium Limited Confidential&amp;B&amp;C&amp;D&amp;RPage &amp;P</oddFooter>
   </headerFooter>
@@ -2986,92 +3053,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6">
-      <c r="B1" s="105" t="s">
+      <c r="B1" s="104" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="104"/>
+      <c r="D1" s="108"/>
+      <c r="E1" s="108"/>
+      <c r="F1" s="108"/>
+    </row>
+    <row r="2" spans="2:6">
+      <c r="B2" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="104"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="105"/>
+      <c r="C3" s="105"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+    </row>
+    <row r="4" spans="2:6" ht="25.5">
+      <c r="B4" s="105" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="105"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="105"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="109"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="109"/>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" s="104" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="104"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="108" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="105"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="109"/>
-      <c r="F1" s="109"/>
-    </row>
-    <row r="2" spans="2:6">
-      <c r="B2" s="105" t="s">
+    </row>
+    <row r="7" spans="2:6" ht="13.5" thickBot="1">
+      <c r="B7" s="105"/>
+      <c r="C7" s="105"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+    </row>
+    <row r="8" spans="2:6" ht="39" thickBot="1">
+      <c r="B8" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-    </row>
-    <row r="3" spans="2:6">
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="110"/>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-    </row>
-    <row r="4" spans="2:6" ht="25.5">
-      <c r="B4" s="106" t="s">
+      <c r="C8" s="107"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110">
+        <v>1</v>
+      </c>
+      <c r="F8" s="111" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="110"/>
-      <c r="E4" s="110"/>
-      <c r="F4" s="110"/>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="110"/>
-      <c r="F5" s="110"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="105" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="105"/>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="109" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="13.5" thickBot="1">
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="110"/>
-      <c r="E7" s="110"/>
-      <c r="F7" s="110"/>
-    </row>
-    <row r="8" spans="2:6" ht="39" thickBot="1">
-      <c r="B8" s="107" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="108"/>
-      <c r="D8" s="111"/>
-      <c r="E8" s="111">
-        <v>1</v>
-      </c>
-      <c r="F8" s="112" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="106"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="109"/>
+      <c r="E9" s="109"/>
+      <c r="F9" s="109"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="106"/>
-      <c r="C10" s="106"/>
-      <c r="D10" s="110"/>
-      <c r="E10" s="110"/>
-      <c r="F10" s="110"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="105"/>
+      <c r="D10" s="109"/>
+      <c r="E10" s="109"/>
+      <c r="F10" s="109"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>